<commit_message>
me stupid adde more changes
</commit_message>
<xml_diff>
--- a/daq_system/inputs/CMS_Master_Data_Wiring_Dev5.xlsx
+++ b/daq_system/inputs/CMS_Master_Data_Wiring_Dev5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nmaso\Documents\DAQ\PSPL_DAQ\daq_system\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89908D23-120C-4B51-BAA4-2E06D866D1D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2813084A-2FC8-46C3-AB49-292B511C653C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2593,7 +2593,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
never using dashes again
</commit_message>
<xml_diff>
--- a/daq_system/inputs/CMS_Master_Data_Wiring_Dev5.xlsx
+++ b/daq_system/inputs/CMS_Master_Data_Wiring_Dev5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nmaso\Documents\DAQ\PSPL_DAQ\daq_system\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910409EF-F097-45E9-BF2A-AFA8463CDC19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF032C9-B077-48D7-9277-3BAE832A7BAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="116">
   <si>
     <t>Name</t>
   </si>
@@ -373,9 +373,6 @@
     <t>TC_FU_02</t>
   </si>
   <si>
-    <t>_773.437</t>
-  </si>
-  <si>
     <t>RTD_OX</t>
   </si>
   <si>
@@ -383,9 +380,6 @@
   </si>
   <si>
     <t>PT_FU_202</t>
-  </si>
-  <si>
-    <t>_5.2730520568402</t>
   </si>
   <si>
     <t>PT_OX_202</t>
@@ -1091,9 +1085,9 @@
   </sheetPr>
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1572,8 +1566,8 @@
       <c r="F12" s="10">
         <v>179.39295000000001</v>
       </c>
-      <c r="G12" s="10" t="s">
-        <v>111</v>
+      <c r="G12" s="10">
+        <v>-773.43700000000001</v>
       </c>
       <c r="H12" s="11">
         <v>0</v>
@@ -1591,7 +1585,7 @@
     </row>
     <row r="13" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>61</v>
@@ -1627,7 +1621,7 @@
     </row>
     <row r="14" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>63</v>
@@ -1663,7 +1657,7 @@
     </row>
     <row r="15" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>64</v>
@@ -1680,8 +1674,8 @@
       <c r="F15" s="17">
         <v>299.727093171143</v>
       </c>
-      <c r="G15" s="17" t="s">
-        <v>115</v>
+      <c r="G15" s="17">
+        <v>-5.2730520568402</v>
       </c>
       <c r="H15" s="11">
         <v>0</v>
@@ -1699,7 +1693,7 @@
     </row>
     <row r="16" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>65</v>
@@ -1714,7 +1708,7 @@
         <v>37</v>
       </c>
       <c r="F16" s="17">
-        <v>300.40325697386402</v>
+        <v>299.727093171143</v>
       </c>
       <c r="G16" s="17">
         <v>2.0020088120354602</v>
@@ -1735,7 +1729,7 @@
     </row>
     <row r="17" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>66</v>
@@ -1750,7 +1744,7 @@
         <v>37</v>
       </c>
       <c r="F17" s="17">
-        <v>22</v>
+        <v>299.727093171143</v>
       </c>
       <c r="G17" s="18">
         <v>93.15</v>
@@ -2597,9 +2591,9 @@
   </sheetPr>
   <dimension ref="A1:U15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
auto changes annd launch sequences V1
</commit_message>
<xml_diff>
--- a/daq_system/inputs/CMS_Master_Data_Wiring_Dev5.xlsx
+++ b/daq_system/inputs/CMS_Master_Data_Wiring_Dev5.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bill\Documents\GitHub\PSPL_DAQ\daq_system\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nmaso\Documents\DAQ\PSPL_DAQ\daq_system\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCDE50F0-FE44-486C-8291-ECC2E7A58367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="1" r:id="rId1"/>
@@ -20,19 +21,6 @@
     <sheet name="DI" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -390,7 +378,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000000"/>
   </numFmts>
@@ -922,7 +910,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -933,15 +921,15 @@
       <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="25" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.73046875" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="25" width="13.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="24" t="s">
         <v>67</v>
       </c>
@@ -972,7 +960,7 @@
       <c r="X1" s="27"/>
       <c r="Y1" s="27"/>
     </row>
-    <row r="2" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>68</v>
       </c>
@@ -980,7 +968,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>69</v>
       </c>
@@ -988,7 +976,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>70</v>
       </c>
@@ -996,7 +984,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>71</v>
       </c>
@@ -1004,7 +992,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>72</v>
       </c>
@@ -1012,7 +1000,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>74</v>
       </c>
@@ -1020,7 +1008,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>76</v>
       </c>
@@ -1028,7 +1016,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>77</v>
       </c>
@@ -1036,7 +1024,7 @@
         <v>10.24</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>78</v>
       </c>
@@ -1044,7 +1032,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>80</v>
       </c>
@@ -1052,7 +1040,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>82</v>
       </c>
@@ -1060,7 +1048,7 @@
         <v>-196</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>83</v>
       </c>
@@ -1078,7 +1066,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1089,25 +1077,25 @@
       <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.73046875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.3984375" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.265625" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.73046875" style="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" style="22" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="13.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.73046875" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.1328125" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.86328125" style="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.86328125" style="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.265625" style="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.1328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="13.59765625" style="19" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1151,7 +1139,7 @@
       <c r="O1" s="27"/>
       <c r="P1" s="27"/>
     </row>
-    <row r="2" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>101</v>
       </c>
@@ -1191,7 +1179,7 @@
       <c r="O2" s="9"/>
       <c r="P2" s="9"/>
     </row>
-    <row r="3" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>102</v>
       </c>
@@ -1231,7 +1219,7 @@
       <c r="O3" s="9"/>
       <c r="P3" s="9"/>
     </row>
-    <row r="4" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>103</v>
       </c>
@@ -1271,7 +1259,7 @@
       <c r="O4" s="9"/>
       <c r="P4" s="9"/>
     </row>
-    <row r="5" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>104</v>
       </c>
@@ -1312,7 +1300,7 @@
       <c r="P5" s="9"/>
       <c r="Q5" s="9"/>
     </row>
-    <row r="6" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>105</v>
       </c>
@@ -1350,7 +1338,7 @@
       <c r="O6" s="9"/>
       <c r="P6" s="9"/>
     </row>
-    <row r="7" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>106</v>
       </c>
@@ -1388,7 +1376,7 @@
       <c r="O7" s="9"/>
       <c r="P7" s="9"/>
     </row>
-    <row r="8" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>107</v>
       </c>
@@ -1428,7 +1416,7 @@
       <c r="O8" s="9"/>
       <c r="P8" s="9"/>
     </row>
-    <row r="9" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>108</v>
       </c>
@@ -1468,7 +1456,7 @@
       <c r="O9" s="9"/>
       <c r="P9" s="9"/>
     </row>
-    <row r="10" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>109</v>
       </c>
@@ -1507,7 +1495,7 @@
       <c r="O10" s="9"/>
       <c r="P10" s="9"/>
     </row>
-    <row r="11" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>110</v>
       </c>
@@ -1546,7 +1534,7 @@
       <c r="O11" s="9"/>
       <c r="P11" s="9"/>
     </row>
-    <row r="12" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>58</v>
       </c>
@@ -1563,7 +1551,7 @@
         <v>37</v>
       </c>
       <c r="F12" s="10">
-        <v>-179.39295000000001</v>
+        <v>179.39295000000001</v>
       </c>
       <c r="G12" s="10">
         <v>-773.43700000000001</v>
@@ -1582,7 +1570,7 @@
       <c r="O12" s="9"/>
       <c r="P12" s="9"/>
     </row>
-    <row r="13" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>111</v>
       </c>
@@ -1618,7 +1606,7 @@
       <c r="O13" s="9"/>
       <c r="P13" s="9"/>
     </row>
-    <row r="14" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>112</v>
       </c>
@@ -1654,7 +1642,7 @@
       <c r="O14" s="9"/>
       <c r="P14" s="9"/>
     </row>
-    <row r="15" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>113</v>
       </c>
@@ -1690,7 +1678,7 @@
       <c r="O15" s="9"/>
       <c r="P15" s="9"/>
     </row>
-    <row r="16" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>114</v>
       </c>
@@ -1726,7 +1714,7 @@
       <c r="O16" s="9"/>
       <c r="P16" s="9"/>
     </row>
-    <row r="17" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
         <v>115</v>
       </c>
@@ -1771,7 +1759,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1782,19 +1770,19 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="26" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="26" width="13.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1845,7 +1833,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1856,22 +1844,22 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="14.73046875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.86328125" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="32" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.59765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.1328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="32" width="13.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1931,7 +1919,7 @@
       <c r="AE1" s="27"/>
       <c r="AF1" s="27"/>
     </row>
-    <row r="2" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1945,7 +1933,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1958,7 +1946,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -1972,7 +1960,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -1985,7 +1973,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -1999,7 +1987,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -2012,7 +2000,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -2026,7 +2014,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -2039,7 +2027,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -2053,7 +2041,7 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -2066,7 +2054,7 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -2080,7 +2068,7 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -2093,7 +2081,7 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -2107,7 +2095,7 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -2120,7 +2108,7 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -2134,7 +2122,7 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -2147,7 +2135,7 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -2161,7 +2149,7 @@
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -2174,7 +2162,7 @@
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
     </row>
-    <row r="20" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -2188,7 +2176,7 @@
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
     </row>
-    <row r="21" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -2201,119 +2189,119 @@
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
     </row>
-    <row r="22" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
     </row>
-    <row r="31" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
     </row>
-    <row r="33" spans="5:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="5:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
     </row>
-    <row r="35" spans="5:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="5:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="5:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
     </row>
-    <row r="38" spans="5:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="5:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
     </row>
-    <row r="40" spans="5:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
     </row>
-    <row r="41" spans="5:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="5:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
@@ -2327,7 +2315,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -2335,22 +2323,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="2" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.86328125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.86328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.86328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.1328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.1328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.73046875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="30" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.1328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="30" width="13.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2404,7 +2392,7 @@
       <c r="AC1" s="27"/>
       <c r="AD1" s="27"/>
     </row>
-    <row r="2" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -2413,7 +2401,7 @@
       <c r="F2" s="3"/>
       <c r="J2" s="3"/>
     </row>
-    <row r="3" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -2422,7 +2410,7 @@
       <c r="F3" s="3"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -2431,7 +2419,7 @@
       <c r="F4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -2440,7 +2428,7 @@
       <c r="F5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -2449,7 +2437,7 @@
       <c r="F6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -2458,7 +2446,7 @@
       <c r="F7" s="3"/>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -2467,7 +2455,7 @@
       <c r="F8" s="3"/>
       <c r="J8" s="3"/>
     </row>
-    <row r="9" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -2476,7 +2464,7 @@
       <c r="F9" s="3"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -2485,7 +2473,7 @@
       <c r="F10" s="3"/>
       <c r="J10" s="3"/>
     </row>
-    <row r="11" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -2494,7 +2482,7 @@
       <c r="F11" s="3"/>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -2503,7 +2491,7 @@
       <c r="F12" s="3"/>
       <c r="J12" s="3"/>
     </row>
-    <row r="13" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -2512,7 +2500,7 @@
       <c r="F13" s="3"/>
       <c r="J13" s="3"/>
     </row>
-    <row r="14" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -2521,7 +2509,7 @@
       <c r="F14" s="3"/>
       <c r="J14" s="3"/>
     </row>
-    <row r="15" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -2530,7 +2518,7 @@
       <c r="F15" s="3"/>
       <c r="J15" s="3"/>
     </row>
-    <row r="16" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -2539,7 +2527,7 @@
       <c r="F16" s="3"/>
       <c r="J16" s="3"/>
     </row>
-    <row r="17" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -2548,7 +2536,7 @@
       <c r="F17" s="3"/>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -2557,7 +2545,7 @@
       <c r="F18" s="3"/>
       <c r="J18" s="3"/>
     </row>
-    <row r="19" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -2566,7 +2554,7 @@
       <c r="F19" s="3"/>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -2584,7 +2572,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -2595,17 +2583,17 @@
       <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="21" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="21" width="13.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2638,7 +2626,7 @@
       <c r="T1" s="27"/>
       <c r="U1" s="27"/>
     </row>
-    <row r="2" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>87</v>
       </c>
@@ -2649,7 +2637,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>88</v>
       </c>
@@ -2660,7 +2648,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>89</v>
       </c>
@@ -2671,7 +2659,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>90</v>
       </c>
@@ -2682,7 +2670,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>91</v>
       </c>
@@ -2693,7 +2681,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>92</v>
       </c>
@@ -2704,7 +2692,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>93</v>
       </c>
@@ -2715,7 +2703,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>94</v>
       </c>
@@ -2726,7 +2714,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>95</v>
       </c>
@@ -2737,7 +2725,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>96</v>
       </c>
@@ -2748,7 +2736,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>97</v>
       </c>
@@ -2759,7 +2747,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>98</v>
       </c>
@@ -2770,7 +2758,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>99</v>
       </c>
@@ -2781,7 +2769,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>100</v>
       </c>

</xml_diff>